<commit_message>
Se agregan fechas de EA2 práctico
</commit_message>
<xml_diff>
--- a/MiCalendario2022.xlsx
+++ b/MiCalendario2022.xlsx
@@ -224,7 +224,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,7 +264,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFABABAB"/>
-        <bgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFBCAAA4"/>
       </patternFill>
     </fill>
     <fill>
@@ -275,8 +275,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFBCAAA4"/>
+        <bgColor rgb="FFABABAB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF777777"/>
-        <bgColor rgb="FF5983B0"/>
+        <bgColor rgb="FF8D6E63"/>
       </patternFill>
     </fill>
     <fill>
@@ -294,7 +300,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF876900"/>
-        <bgColor rgb="FF777777"/>
+        <bgColor rgb="FF8D6E63"/>
       </patternFill>
     </fill>
     <fill>
@@ -312,7 +318,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBA55D3"/>
-        <bgColor rgb="FFDB287A"/>
+        <bgColor rgb="FF8D6E63"/>
       </patternFill>
     </fill>
     <fill>
@@ -347,8 +353,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF8D6E63"/>
+        <bgColor rgb="FF777777"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF4E342E"/>
-        <bgColor rgb="FF1B1B1B"/>
+        <bgColor rgb="FF6D4C41"/>
       </patternFill>
     </fill>
     <fill>
@@ -391,6 +403,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6D4C41"/>
+        <bgColor rgb="FF4E342E"/>
       </patternFill>
     </fill>
   </fills>
@@ -477,7 +495,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -558,7 +576,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -566,7 +588,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -574,7 +596,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -594,11 +616,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -606,15 +624,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -622,15 +644,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="18" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,15 +656,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="20" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="20" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="21" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -654,7 +676,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="21" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="23" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -670,15 +696,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="22" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="24" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,24 +708,40 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="27" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="28" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="27" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="28" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="29" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="30" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="31" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -754,7 +788,7 @@
       <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF777777"/>
       <rgbColor rgb="FF729FCF"/>
-      <rgbColor rgb="FFDB287A"/>
+      <rgbColor rgb="FF6D4C41"/>
       <rgbColor rgb="FFFAFAFA"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -775,9 +809,9 @@
       <rgbColor rgb="FFFDE9A9"/>
       <rgbColor rgb="FF9BD1CB"/>
       <rgbColor rgb="FFFFB66C"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFBCAAA4"/>
       <rgbColor rgb="FFFFDBB6"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FFBA55D3"/>
       <rgbColor rgb="FF669A95"/>
       <rgbColor rgb="FF92E285"/>
       <rgbColor rgb="FFE9B913"/>
@@ -790,8 +824,8 @@
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF1B1B1B"/>
       <rgbColor rgb="FF8D281E"/>
-      <rgbColor rgb="FFBA55D3"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FFDB287A"/>
+      <rgbColor rgb="FF8D6E63"/>
       <rgbColor rgb="FF4E342E"/>
     </indexedColors>
   </colors>
@@ -805,8 +839,8 @@
   </sheetPr>
   <dimension ref="B1:AW38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AS28" activeCellId="0" sqref="AS28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S19" activeCellId="0" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1390,7 +1424,7 @@
       <c r="AC8" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="AD8" s="14" t="n">
+      <c r="AD8" s="20" t="n">
         <v>18</v>
       </c>
       <c r="AE8" s="14" t="n">
@@ -1483,52 +1517,52 @@
         <v>30</v>
       </c>
       <c r="AJ9" s="0"/>
-      <c r="AN9" s="20" t="s">
+      <c r="AN9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="AO9" s="20"/>
-      <c r="AP9" s="20"/>
-      <c r="AQ9" s="20"/>
-      <c r="AR9" s="20"/>
-      <c r="AS9" s="21"/>
+      <c r="AO9" s="21"/>
+      <c r="AP9" s="21"/>
+      <c r="AQ9" s="21"/>
+      <c r="AR9" s="21"/>
+      <c r="AS9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="13" t="n">
         <v>31</v>
       </c>
       <c r="I10" s="0"/>
-      <c r="AN10" s="22" t="s">
+      <c r="AN10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="AO10" s="23"/>
-      <c r="AP10" s="24" t="s">
+      <c r="AO10" s="24"/>
+      <c r="AP10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="AQ10" s="23"/>
-      <c r="AR10" s="25" t="s">
+      <c r="AQ10" s="24"/>
+      <c r="AR10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="AS10" s="26" t="s">
+      <c r="AS10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AT10" s="26"/>
-      <c r="AU10" s="26"/>
-      <c r="AV10" s="26"/>
-      <c r="AW10" s="26"/>
+      <c r="AT10" s="27"/>
+      <c r="AU10" s="27"/>
+      <c r="AV10" s="27"/>
+      <c r="AW10" s="27"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AN11" s="27"/>
-      <c r="AR11" s="28"/>
+      <c r="AN11" s="28"/>
+      <c r="AR11" s="29"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AN12" s="20" t="s">
+      <c r="AN12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AO12" s="20"/>
-      <c r="AP12" s="20"/>
-      <c r="AQ12" s="20"/>
-      <c r="AR12" s="20"/>
-      <c r="AS12" s="21"/>
+      <c r="AO12" s="21"/>
+      <c r="AP12" s="21"/>
+      <c r="AQ12" s="21"/>
+      <c r="AR12" s="21"/>
+      <c r="AS12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
@@ -1567,22 +1601,22 @@
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
       <c r="AJ13" s="6"/>
-      <c r="AN13" s="29" t="s">
+      <c r="AN13" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="AO13" s="23"/>
-      <c r="AP13" s="30"/>
-      <c r="AQ13" s="23"/>
-      <c r="AR13" s="31" t="s">
+      <c r="AO13" s="24"/>
+      <c r="AP13" s="31"/>
+      <c r="AQ13" s="24"/>
+      <c r="AR13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="AS13" s="26" t="s">
+      <c r="AS13" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AT13" s="26"/>
-      <c r="AU13" s="26"/>
-      <c r="AV13" s="26"/>
-      <c r="AW13" s="26"/>
+      <c r="AT13" s="27"/>
+      <c r="AU13" s="27"/>
+      <c r="AV13" s="27"/>
+      <c r="AW13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
@@ -1681,8 +1715,8 @@
       <c r="AJ14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AN14" s="27"/>
-      <c r="AR14" s="28"/>
+      <c r="AN14" s="28"/>
+      <c r="AR14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="n">
@@ -1701,7 +1735,7 @@
         <v>19</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="32"/>
+      <c r="M15" s="33"/>
       <c r="N15" s="17" t="n">
         <v>1</v>
       </c>
@@ -1721,10 +1755,10 @@
         <v>23</v>
       </c>
       <c r="U15" s="4"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="33" t="n">
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="34" t="n">
         <v>1</v>
       </c>
       <c r="Z15" s="17" t="n">
@@ -1748,7 +1782,7 @@
       <c r="AG15" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="AH15" s="34" t="n">
+      <c r="AH15" s="35" t="n">
         <v>5</v>
       </c>
       <c r="AI15" s="17" t="n">
@@ -1757,14 +1791,14 @@
       <c r="AJ15" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="AN15" s="35" t="s">
+      <c r="AN15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="AO15" s="35"/>
-      <c r="AP15" s="35"/>
-      <c r="AQ15" s="35"/>
-      <c r="AR15" s="35"/>
-      <c r="AS15" s="21"/>
+      <c r="AO15" s="36"/>
+      <c r="AP15" s="36"/>
+      <c r="AQ15" s="36"/>
+      <c r="AR15" s="36"/>
+      <c r="AS15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="n">
@@ -1842,7 +1876,7 @@
       <c r="AC16" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="AD16" s="36" t="n">
+      <c r="AD16" s="37" t="n">
         <v>8</v>
       </c>
       <c r="AE16" s="17" t="n">
@@ -1863,18 +1897,18 @@
       <c r="AJ16" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="AN16" s="37" t="s">
+      <c r="AN16" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="AO16" s="23"/>
-      <c r="AP16" s="38" t="s">
+      <c r="AO16" s="24"/>
+      <c r="AP16" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="AQ16" s="23"/>
-      <c r="AR16" s="39" t="s">
+      <c r="AQ16" s="24"/>
+      <c r="AR16" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="AS16" s="40"/>
+      <c r="AS16" s="41"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="n">
@@ -1928,7 +1962,7 @@
       <c r="T17" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="U17" s="41" t="n">
+      <c r="U17" s="42" t="n">
         <v>11</v>
       </c>
       <c r="V17" s="13" t="n">
@@ -1937,7 +1971,7 @@
       <c r="W17" s="13" t="n">
         <v>13</v>
       </c>
-      <c r="X17" s="42" t="n">
+      <c r="X17" s="43" t="n">
         <v>14</v>
       </c>
       <c r="Y17" s="13" t="n">
@@ -1964,7 +1998,7 @@
       <c r="AG17" s="17" t="n">
         <v>18</v>
       </c>
-      <c r="AH17" s="34" t="n">
+      <c r="AH17" s="35" t="n">
         <v>19</v>
       </c>
       <c r="AI17" s="17" t="n">
@@ -1973,8 +2007,8 @@
       <c r="AJ17" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="AN17" s="27"/>
-      <c r="AR17" s="28"/>
+      <c r="AN17" s="28"/>
+      <c r="AR17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
@@ -2010,7 +2044,7 @@
       <c r="M18" s="17" t="n">
         <v>21</v>
       </c>
-      <c r="N18" s="29" t="n">
+      <c r="N18" s="30" t="n">
         <v>22</v>
       </c>
       <c r="O18" s="18" t="n">
@@ -2037,10 +2071,10 @@
       <c r="W18" s="13" t="n">
         <v>20</v>
       </c>
-      <c r="X18" s="42" t="n">
+      <c r="X18" s="43" t="n">
         <v>21</v>
       </c>
-      <c r="Y18" s="43" t="n">
+      <c r="Y18" s="44" t="n">
         <v>22</v>
       </c>
       <c r="Z18" s="17" t="n">
@@ -2073,14 +2107,14 @@
       <c r="AJ18" s="9" t="n">
         <v>28</v>
       </c>
-      <c r="AN18" s="35" t="s">
+      <c r="AN18" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="AO18" s="35"/>
-      <c r="AP18" s="35"/>
-      <c r="AQ18" s="35"/>
-      <c r="AR18" s="35"/>
-      <c r="AS18" s="21"/>
+      <c r="AO18" s="36"/>
+      <c r="AP18" s="36"/>
+      <c r="AQ18" s="36"/>
+      <c r="AR18" s="36"/>
+      <c r="AS18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
@@ -2110,16 +2144,16 @@
       <c r="K19" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="L19" s="17" t="n">
+      <c r="L19" s="45" t="n">
         <v>27</v>
       </c>
       <c r="M19" s="17" t="n">
         <v>28</v>
       </c>
-      <c r="N19" s="44" t="n">
+      <c r="N19" s="46" t="n">
         <v>29</v>
       </c>
-      <c r="O19" s="45" t="n">
+      <c r="O19" s="47" t="n">
         <v>30</v>
       </c>
       <c r="P19" s="4"/>
@@ -2137,7 +2171,7 @@
       <c r="W19" s="13" t="n">
         <v>27</v>
       </c>
-      <c r="X19" s="42" t="n">
+      <c r="X19" s="43" t="n">
         <v>28</v>
       </c>
       <c r="Y19" s="13" t="n">
@@ -2161,22 +2195,22 @@
       <c r="AF19" s="17" t="n">
         <v>31</v>
       </c>
-      <c r="AG19" s="46"/>
-      <c r="AH19" s="46"/>
-      <c r="AI19" s="47"/>
+      <c r="AG19" s="48"/>
+      <c r="AH19" s="48"/>
+      <c r="AI19" s="49"/>
       <c r="AJ19" s="0"/>
-      <c r="AN19" s="48" t="s">
+      <c r="AN19" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AO19" s="23"/>
-      <c r="AP19" s="49" t="s">
+      <c r="AO19" s="24"/>
+      <c r="AP19" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="AQ19" s="23"/>
-      <c r="AR19" s="50" t="s">
+      <c r="AQ19" s="24"/>
+      <c r="AR19" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="AS19" s="40"/>
+      <c r="AS19" s="41"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="n">
@@ -2188,42 +2222,42 @@
       <c r="D20" s="17" t="n">
         <v>31</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
       <c r="U20" s="0"/>
       <c r="AA20" s="0"/>
-      <c r="AN20" s="27"/>
-      <c r="AR20" s="28"/>
+      <c r="AN20" s="28"/>
+      <c r="AR20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AN21" s="20" t="s">
+      <c r="AN21" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AO21" s="20"/>
-      <c r="AP21" s="20"/>
-      <c r="AQ21" s="20"/>
-      <c r="AR21" s="20"/>
-      <c r="AS21" s="21"/>
+      <c r="AO21" s="21"/>
+      <c r="AP21" s="21"/>
+      <c r="AQ21" s="21"/>
+      <c r="AR21" s="21"/>
+      <c r="AS21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AN22" s="36" t="s">
+      <c r="AN22" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="AO22" s="23"/>
-      <c r="AP22" s="51"/>
-      <c r="AQ22" s="23"/>
-      <c r="AR22" s="52" t="s">
+      <c r="AO22" s="24"/>
+      <c r="AP22" s="53"/>
+      <c r="AQ22" s="24"/>
+      <c r="AR22" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="AS22" s="26" t="s">
+      <c r="AS22" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AT22" s="26"/>
-      <c r="AU22" s="26"/>
-      <c r="AV22" s="26"/>
-      <c r="AW22" s="26"/>
+      <c r="AT22" s="27"/>
+      <c r="AU22" s="27"/>
+      <c r="AV22" s="27"/>
+      <c r="AW22" s="27"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="6" t="s">
@@ -2262,8 +2296,8 @@
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="AJ23" s="6"/>
-      <c r="AN23" s="27"/>
-      <c r="AR23" s="28"/>
+      <c r="AN23" s="28"/>
+      <c r="AR23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
@@ -2362,14 +2396,14 @@
       <c r="AJ24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AN24" s="20" t="s">
+      <c r="AN24" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="AO24" s="20"/>
-      <c r="AP24" s="20"/>
-      <c r="AQ24" s="20"/>
-      <c r="AR24" s="20"/>
-      <c r="AS24" s="21"/>
+      <c r="AO24" s="21"/>
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="21"/>
+      <c r="AR24" s="21"/>
+      <c r="AS24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="n">
@@ -2390,10 +2424,10 @@
       <c r="K25" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="M25" s="53"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
-      <c r="P25" s="53"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
       <c r="Q25" s="14" t="n">
         <v>1</v>
       </c>
@@ -2407,7 +2441,7 @@
       <c r="V25" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="W25" s="44" t="n">
+      <c r="W25" s="46" t="n">
         <v>2</v>
       </c>
       <c r="X25" s="18" t="n">
@@ -2425,7 +2459,7 @@
       <c r="AC25" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="AG25" s="42" t="n">
+      <c r="AG25" s="43" t="n">
         <v>1</v>
       </c>
       <c r="AH25" s="14" t="n">
@@ -2437,22 +2471,22 @@
       <c r="AJ25" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="AN25" s="54" t="s">
+      <c r="AN25" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="AO25" s="23"/>
-      <c r="AP25" s="55"/>
-      <c r="AQ25" s="23"/>
-      <c r="AR25" s="56" t="s">
+      <c r="AO25" s="24"/>
+      <c r="AP25" s="57"/>
+      <c r="AQ25" s="24"/>
+      <c r="AR25" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="AS25" s="57" t="s">
+      <c r="AS25" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="AT25" s="57"/>
-      <c r="AU25" s="57"/>
-      <c r="AV25" s="57"/>
-      <c r="AW25" s="57"/>
+      <c r="AT25" s="59"/>
+      <c r="AU25" s="59"/>
+      <c r="AV25" s="59"/>
+      <c r="AW25" s="59"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="n">
@@ -2470,7 +2504,7 @@
       <c r="F26" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="29" t="n">
+      <c r="G26" s="30" t="n">
         <v>9</v>
       </c>
       <c r="H26" s="17" t="n">
@@ -2506,19 +2540,19 @@
       <c r="T26" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="U26" s="17" t="n">
+      <c r="U26" s="45" t="n">
         <v>7</v>
       </c>
       <c r="V26" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="W26" s="44" t="n">
+      <c r="W26" s="46" t="n">
         <v>9</v>
       </c>
-      <c r="X26" s="42" t="n">
+      <c r="X26" s="43" t="n">
         <v>10</v>
       </c>
-      <c r="Y26" s="29" t="n">
+      <c r="Y26" s="30" t="n">
         <v>11</v>
       </c>
       <c r="Z26" s="14" t="n">
@@ -2530,7 +2564,7 @@
       <c r="AC26" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="AD26" s="41" t="n">
+      <c r="AD26" s="42" t="n">
         <v>5</v>
       </c>
       <c r="AE26" s="14" t="n">
@@ -2551,8 +2585,8 @@
       <c r="AJ26" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="AN26" s="27"/>
-      <c r="AR26" s="28"/>
+      <c r="AN26" s="28"/>
+      <c r="AR26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="n">
@@ -2606,7 +2640,7 @@
       <c r="T27" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="U27" s="36" t="n">
+      <c r="U27" s="37" t="n">
         <v>14</v>
       </c>
       <c r="V27" s="17" t="n">
@@ -2615,7 +2649,7 @@
       <c r="W27" s="17" t="n">
         <v>16</v>
       </c>
-      <c r="X27" s="42" t="n">
+      <c r="X27" s="43" t="n">
         <v>17</v>
       </c>
       <c r="Y27" s="17" t="n">
@@ -2630,7 +2664,7 @@
       <c r="AC27" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="AD27" s="41" t="n">
+      <c r="AD27" s="42" t="n">
         <v>12</v>
       </c>
       <c r="AE27" s="14" t="n">
@@ -2639,7 +2673,7 @@
       <c r="AF27" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="AG27" s="42" t="n">
+      <c r="AG27" s="43" t="n">
         <v>15</v>
       </c>
       <c r="AH27" s="19" t="n">
@@ -2651,13 +2685,13 @@
       <c r="AJ27" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="AN27" s="20" t="s">
+      <c r="AN27" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AO27" s="20"/>
-      <c r="AP27" s="20"/>
-      <c r="AQ27" s="20"/>
-      <c r="AR27" s="20"/>
+      <c r="AO27" s="21"/>
+      <c r="AP27" s="21"/>
+      <c r="AQ27" s="21"/>
+      <c r="AR27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="n">
@@ -2720,7 +2754,7 @@
       <c r="W28" s="17" t="n">
         <v>23</v>
       </c>
-      <c r="X28" s="42" t="n">
+      <c r="X28" s="43" t="n">
         <v>24</v>
       </c>
       <c r="Y28" s="17" t="n">
@@ -2735,7 +2769,7 @@
       <c r="AC28" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="AD28" s="45" t="n">
+      <c r="AD28" s="47" t="n">
         <v>19</v>
       </c>
       <c r="AE28" s="14" t="n">
@@ -2756,24 +2790,24 @@
       <c r="AJ28" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="AN28" s="44" t="s">
+      <c r="AN28" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="AO28" s="45"/>
-      <c r="AP28" s="45" t="s">
+      <c r="AO28" s="47"/>
+      <c r="AP28" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="AQ28" s="45"/>
-      <c r="AR28" s="45" t="s">
+      <c r="AQ28" s="47"/>
+      <c r="AR28" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="AS28" s="58" t="s">
+      <c r="AS28" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="AT28" s="58"/>
-      <c r="AU28" s="58"/>
-      <c r="AV28" s="58"/>
-      <c r="AW28" s="58"/>
+      <c r="AT28" s="62"/>
+      <c r="AU28" s="62"/>
+      <c r="AV28" s="62"/>
+      <c r="AW28" s="62"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="n">
@@ -2794,7 +2828,7 @@
       <c r="G29" s="12" t="n">
         <v>30</v>
       </c>
-      <c r="H29" s="32"/>
+      <c r="H29" s="33"/>
       <c r="I29" s="0"/>
       <c r="K29" s="2" t="n">
         <v>40</v>
@@ -2811,7 +2845,7 @@
       <c r="O29" s="17" t="n">
         <v>27</v>
       </c>
-      <c r="P29" s="29" t="n">
+      <c r="P29" s="30" t="n">
         <v>28</v>
       </c>
       <c r="Q29" s="17" t="n">
@@ -2823,7 +2857,7 @@
       <c r="T29" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="U29" s="41" t="n">
+      <c r="U29" s="42" t="n">
         <v>28</v>
       </c>
       <c r="V29" s="17" t="n">
@@ -2858,19 +2892,19 @@
         <v>31</v>
       </c>
       <c r="AJ29" s="0"/>
-      <c r="AN29" s="59"/>
-      <c r="AO29" s="60"/>
-      <c r="AP29" s="60"/>
-      <c r="AQ29" s="60"/>
-      <c r="AR29" s="61"/>
+      <c r="AN29" s="63"/>
+      <c r="AO29" s="64"/>
+      <c r="AP29" s="64"/>
+      <c r="AQ29" s="64"/>
+      <c r="AR29" s="65"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
       <c r="K30" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="L30" s="36" t="n">
+      <c r="L30" s="37" t="n">
         <v>31</v>
       </c>
       <c r="M30" s="4"/>

</xml_diff>